<commit_message>
corrigiendo nro de cuenta
</commit_message>
<xml_diff>
--- a/docs/componentes/Descripcion_de_Bungalows.xlsx
+++ b/docs/componentes/Descripcion_de_Bungalows.xlsx
@@ -86,9 +86,6 @@
     <t>Ambas con ventilador y baño completo y teléfono.</t>
   </si>
   <si>
-    <t xml:space="preserve">BUNGALOW CLÁSICO : 31 A - 31 B </t>
-  </si>
-  <si>
     <t>Ubicación: sobre la playa pero sin vista al mar</t>
   </si>
   <si>
@@ -377,6 +374,22 @@
   </si>
   <si>
     <t>Capacidad mínima 8 personas, capacidad máxima 11 personas.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BUNGALOW CLÁSICO : 31 A - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">31 B </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -790,7 +803,7 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -800,7 +813,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -817,7 +830,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -834,14 +847,14 @@
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -851,7 +864,7 @@
     </row>
     <row r="5" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -859,7 +872,7 @@
       <c r="E5" s="2"/>
       <c r="G5" s="10"/>
       <c r="H5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -873,10 +886,10 @@
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -960,14 +973,14 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="H19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="13"/>
@@ -977,14 +990,14 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="H20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1007,14 +1020,14 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="H22" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -1099,7 +1112,7 @@
     </row>
     <row r="34" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1108,7 +1121,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="6"/>
       <c r="H34" s="1" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -1118,7 +1131,7 @@
     </row>
     <row r="35" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1127,7 +1140,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="6"/>
       <c r="H35" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1141,26 +1154,26 @@
     </row>
     <row r="37" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1168,10 +1181,10 @@
         <v>18</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1179,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1209,7 +1222,7 @@
     </row>
     <row r="46" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1217,7 +1230,7 @@
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="H46" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -1227,7 +1240,7 @@
     </row>
     <row r="47" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1235,7 +1248,7 @@
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="H47" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -1257,14 +1270,14 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="H49" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
@@ -1273,42 +1286,42 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1333,7 +1346,7 @@
     </row>
     <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -1341,7 +1354,7 @@
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="H58" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -1351,7 +1364,7 @@
     </row>
     <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -1359,7 +1372,7 @@
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
       <c r="H59" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -1378,10 +1391,10 @@
     </row>
     <row r="61" spans="1:13" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
@@ -1391,39 +1404,39 @@
     </row>
     <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H66" s="4" t="s">
         <v>9</v>
@@ -1431,7 +1444,7 @@
     </row>
     <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H67" s="4" t="s">
         <v>10</v>
@@ -1442,7 +1455,7 @@
     </row>
     <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -1452,7 +1465,7 @@
     </row>
     <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -1470,7 +1483,7 @@
     </row>
     <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1481,12 +1494,12 @@
     </row>
     <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
actualizando archivo de habitaciones
</commit_message>
<xml_diff>
--- a/docs/componentes/Descripcion_de_Bungalows.xlsx
+++ b/docs/componentes/Descripcion_de_Bungalows.xlsx
@@ -377,7 +377,28 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">BUNGALOW CLÁSICO : 31 A - </t>
+      <t xml:space="preserve">BUNGALOW CLÁSICO : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>31 A</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
     </r>
     <r>
       <rPr>
@@ -802,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
cambios en el programa
</commit_message>
<xml_diff>
--- a/docs/componentes/Descripcion_de_Bungalows.xlsx
+++ b/docs/componentes/Descripcion_de_Bungalows.xlsx
@@ -385,7 +385,7 @@
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">- </t>
+      <t>- 6 - 7 - 8 -</t>
     </r>
     <r>
       <rPr>
@@ -396,17 +396,22 @@
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">6 - 7 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>- 8 -</t>
+      <t xml:space="preserve"> 9 - 14 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>- 15 - 16 - 17 -18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HABITACIÓN CON VISTA A LA PISCINA </t>
     </r>
     <r>
       <rPr>
@@ -417,17 +422,17 @@
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> 9 - </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>14 -</t>
+      <t>19 20 21</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 22 23 24</t>
     </r>
     <r>
       <rPr>
@@ -438,43 +443,17 @@
         <rFont val="Cambria"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> 15</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - 16 - 17 -18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">HABITACIÓN CON VISTA A LA PISCINA DE </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <strike/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t>19</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Cambria"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> A 30 </t>
+      <t xml:space="preserve"> 25 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Cambria"/>
+        <family val="1"/>
+      </rPr>
+      <t>26 27 28 29 30</t>
     </r>
   </si>
 </sst>
@@ -897,7 +876,7 @@
   <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+      <selection activeCell="L67" sqref="L67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1364,7 +1343,7 @@
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>67</v>
       </c>
@@ -1380,7 +1359,7 @@
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>27</v>
       </c>
@@ -1388,7 +1367,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>29</v>
       </c>
@@ -1396,7 +1375,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -1404,7 +1383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>33</v>
       </c>
@@ -1412,7 +1391,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>35</v>
       </c>
@@ -1420,7 +1399,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>9</v>
       </c>
@@ -1428,7 +1407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>10</v>
       </c>
@@ -1436,11 +1415,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
         <v>37</v>
       </c>
@@ -1457,8 +1436,9 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
       <c r="M58" s="2"/>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>52</v>
       </c>
@@ -1475,8 +1455,9 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
       <c r="M59" s="2"/>
-    </row>
-    <row r="60" spans="1:13" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="H60" s="4"/>
       <c r="I60" s="3"/>
@@ -1485,7 +1466,7 @@
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="1:13" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>68</v>
       </c>
@@ -1498,7 +1479,7 @@
       <c r="L61" s="3"/>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>38</v>
       </c>
@@ -1506,7 +1487,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>39</v>
       </c>
@@ -1514,7 +1495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>41</v>
       </c>

</xml_diff>